<commit_message>
update callback filtre resp_com
</commit_message>
<xml_diff>
--- a/appPCOE/src/tableau_calcul_evolution_prix.xlsx
+++ b/appPCOE/src/tableau_calcul_evolution_prix.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SofianOUASS\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SofianOUASS\Documents\Dev\app-pcoe\appPCOE\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0AEB1CF4-B094-4C80-9885-CC38651E9A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1BA093-72B6-498F-9696-F206A3CDA293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4F30396C-89AD-4EC6-9E7A-106189CB70E9}"/>
   </bookViews>
@@ -36,14 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Coeff évol prix achat SAP Paper</t>
-  </si>
-  <si>
-    <t>Coefficient annuel
-01/01 au 31/12
-(date anniv contrat)</t>
   </si>
   <si>
     <t>Coeff évol prix achat SAP BOBJ</t>
@@ -85,7 +80,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -108,29 +103,14 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -446,70 +426,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D827F117-7FCC-41B6-8E75-4591E5D4A091}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29.77734375" customWidth="1"/>
     <col min="2" max="2" width="12.44140625" customWidth="1"/>
-    <col min="3" max="3" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2">
         <v>0.06</v>
       </c>
-      <c r="C1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="B2" s="2">
         <v>0.08</v>
       </c>
-      <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2">
         <v>0.02</v>
       </c>
-      <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2">
         <v>0.05</v>
       </c>
-      <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
         <v>0</v>
       </c>
-      <c r="C5" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C1:C5"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>